<commit_message>
commiting datasets for Rmd analysis
</commit_message>
<xml_diff>
--- a/offender_data/offender_2014-18.xlsx
+++ b/offender_data/offender_2014-18.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guestuser/death_row/offender_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F96D63-094A-0B40-A646-2921A11EDDC3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49164DFD-E737-0449-B8F8-A7BA7B976F80}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="26840" windowHeight="15540" xr2:uid="{7DDCCF7A-F144-F547-AA5E-684F202E0CCD}"/>
+    <workbookView xWindow="6100" yWindow="460" windowWidth="26840" windowHeight="15540" xr2:uid="{7DDCCF7A-F144-F547-AA5E-684F202E0CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="303">
   <si>
     <t>Execution</t>
   </si>
@@ -607,12 +608,366 @@
   <si>
     <t xml:space="preserve">  To everyone that has been there for me you know who you are.  Love y’all.  See y’all on the other side. That’s it.</t>
   </si>
+  <si>
+    <t>Last Statement</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>McCoskey</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>Yowell</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>Feldman</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>Quintanilla</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>McCarthy</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Chester</t>
+  </si>
+  <si>
+    <t>Elroy</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Jeffrey</t>
+  </si>
+  <si>
+    <t>Parr</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>McLennan</t>
+  </si>
+  <si>
+    <t>Cobb</t>
+  </si>
+  <si>
+    <t>Cherokee</t>
+  </si>
+  <si>
+    <t>Threadgill</t>
+  </si>
+  <si>
+    <t>Ronnie</t>
+  </si>
+  <si>
+    <t>Navarro</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>Rickey</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Brazos</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>Preston</t>
+  </si>
+  <si>
+    <t>Ramon</t>
+  </si>
+  <si>
+    <t>Swain</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Gregg</t>
+  </si>
+  <si>
+    <t>Roberts, Jr.</t>
+  </si>
+  <si>
+    <t>Donnie</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>Hines</t>
+  </si>
+  <si>
+    <t>Bobby</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
+  </si>
+  <si>
+    <t>Foster</t>
+  </si>
+  <si>
+    <t>Cleve</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>Hearn</t>
+  </si>
+  <si>
+    <t>Yokamon</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Beunka</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Thurmond</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>Rivas</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Esparza</t>
+  </si>
+  <si>
+    <t>Guadalupe</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Brewer</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Woods</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Denton</t>
+  </si>
+  <si>
+    <t>Robles</t>
+  </si>
+  <si>
+    <t>Stroman</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Leal</t>
+  </si>
+  <si>
+    <t>Humberto</t>
+  </si>
+  <si>
+    <t>Mathis</t>
+  </si>
+  <si>
+    <t>Milton</t>
+  </si>
+  <si>
+    <t>Fort Bend</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Bowie</t>
+  </si>
+  <si>
+    <t>Bradford</t>
+  </si>
+  <si>
+    <t>Gayland</t>
+  </si>
+  <si>
+    <t>Cary</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Wooten</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>Cantu</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Powell</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Travis</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Cannady</t>
+  </si>
+  <si>
+    <t>Rogelio</t>
+  </si>
+  <si>
+    <t>Galloway</t>
+  </si>
+  <si>
+    <t>Billy</t>
+  </si>
+  <si>
+    <t>Varga</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Bustamante</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Berkley</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>Alix</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Sigala</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Gary</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -647,6 +1002,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -669,7 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -680,6 +1042,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -995,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2829B7F3-B83F-BB43-894E-419A4E2C706B}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:N109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,7 +1624,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>549</v>
       </c>
@@ -2562,8 +2926,1643 @@
         <v>164</v>
       </c>
     </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>508</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E50" s="1">
+        <v>43</v>
+      </c>
+      <c r="F50" s="3">
+        <v>41611</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>507</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" s="1">
+        <v>49</v>
+      </c>
+      <c r="F51" s="3">
+        <v>41590</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>506</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E52" s="1">
+        <v>43</v>
+      </c>
+      <c r="F52" s="3">
+        <v>41556</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>505</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E53" s="1">
+        <v>37</v>
+      </c>
+      <c r="F53" s="3">
+        <v>41543</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>504</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="1">
+        <v>30</v>
+      </c>
+      <c r="F54" s="3">
+        <v>41536</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>503</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E55" s="1">
+        <v>55</v>
+      </c>
+      <c r="F55" s="3">
+        <v>41486</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>502</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E56" s="1">
+        <v>41</v>
+      </c>
+      <c r="F56" s="3">
+        <v>41473</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>501</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="1">
+        <v>36</v>
+      </c>
+      <c r="F57" s="3">
+        <v>41471</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>500</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E58" s="1">
+        <v>52</v>
+      </c>
+      <c r="F58" s="3">
+        <v>41451</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>499</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E59" s="1">
+        <v>43</v>
+      </c>
+      <c r="F59" s="3">
+        <v>41437</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>498</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="1">
+        <v>37</v>
+      </c>
+      <c r="F60" s="3">
+        <v>41409</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>497</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E61" s="1">
+        <v>35</v>
+      </c>
+      <c r="F61" s="3">
+        <v>41401</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>496</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="1">
+        <v>29</v>
+      </c>
+      <c r="F62" s="3">
+        <v>41389</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>495</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E63" s="1">
+        <v>40</v>
+      </c>
+      <c r="F63" s="3">
+        <v>41380</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>494</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E64" s="1">
+        <v>50</v>
+      </c>
+      <c r="F64" s="3">
+        <v>41373</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>493</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E65" s="1">
+        <v>48</v>
+      </c>
+      <c r="F65" s="3">
+        <v>41326</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>492</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" s="1">
+        <v>46</v>
+      </c>
+      <c r="F66" s="3">
+        <v>41228</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>491</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E67" s="1">
+        <v>41</v>
+      </c>
+      <c r="F67" s="3">
+        <v>41227</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N67" s="9"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>490</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E68" s="1">
+        <v>33</v>
+      </c>
+      <c r="F68" s="3">
+        <v>41221</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>489</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E69" s="1">
+        <v>41</v>
+      </c>
+      <c r="F69" s="3">
+        <v>41213</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>488</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E70" s="1">
+        <v>40</v>
+      </c>
+      <c r="F70" s="3">
+        <v>41206</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>487</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E71" s="1">
+        <v>44</v>
+      </c>
+      <c r="F71" s="3">
+        <v>41192</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>486</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E72" s="1">
+        <v>48</v>
+      </c>
+      <c r="F72" s="3">
+        <v>41177</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>485</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="1">
+        <v>40</v>
+      </c>
+      <c r="F73" s="3">
+        <v>41172</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>484</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E74" s="1">
+        <v>54</v>
+      </c>
+      <c r="F74" s="3">
+        <v>41128</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>483</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E75" s="1">
+        <v>33</v>
+      </c>
+      <c r="F75" s="3">
+        <v>41108</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>482</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E76" s="1">
+        <v>29</v>
+      </c>
+      <c r="F76" s="3">
+        <v>41025</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>481</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E77" s="1">
+        <v>47</v>
+      </c>
+      <c r="F77" s="3">
+        <v>40996</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>480</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E78" s="1">
+        <v>52</v>
+      </c>
+      <c r="F78" s="3">
+        <v>40975</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>479</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E79" s="1">
+        <v>41</v>
+      </c>
+      <c r="F79" s="3">
+        <v>40968</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>478</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E80" s="1">
+        <v>38</v>
+      </c>
+      <c r="F80" s="3">
+        <v>40934</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>477</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E81" s="1">
+        <v>46</v>
+      </c>
+      <c r="F81" s="3">
+        <v>40863</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>476</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E82" s="1">
+        <v>39</v>
+      </c>
+      <c r="F82" s="3">
+        <v>40843</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>475</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E83" s="1">
+        <v>44</v>
+      </c>
+      <c r="F83" s="3">
+        <v>40807</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>474</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E84" s="1">
+        <v>31</v>
+      </c>
+      <c r="F84" s="3">
+        <v>40799</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>473</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E85" s="1">
+        <v>33</v>
+      </c>
+      <c r="F85" s="3">
+        <v>40765</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>472</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E86" s="1">
+        <v>42</v>
+      </c>
+      <c r="F86" s="3">
+        <v>40744</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>471</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E87" s="1">
+        <v>38</v>
+      </c>
+      <c r="F87" s="3">
+        <v>40731</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>470</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E88" s="1">
+        <v>32</v>
+      </c>
+      <c r="F88" s="3">
+        <v>40715</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>469</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E89" s="1">
+        <v>32</v>
+      </c>
+      <c r="F89" s="3">
+        <v>40710</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>468</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E90" s="1">
+        <v>42</v>
+      </c>
+      <c r="F90" s="3">
+        <v>40695</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>467</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E91" s="1">
+        <v>46</v>
+      </c>
+      <c r="F91" s="3">
+        <v>40666</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>466</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E92" s="1">
+        <v>42</v>
+      </c>
+      <c r="F92" s="3">
+        <v>40596</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>465</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E93" s="1">
+        <v>31</v>
+      </c>
+      <c r="F93" s="3">
+        <v>40589</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>464</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E94" s="1">
+        <v>51</v>
+      </c>
+      <c r="F94" s="3">
+        <v>40472</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>463</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E95" s="1">
+        <v>35</v>
+      </c>
+      <c r="F95" s="3">
+        <v>40407</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>462</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="1">
+        <v>42</v>
+      </c>
+      <c r="F96" s="3">
+        <v>40379</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>461</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E97" s="1">
+        <v>28</v>
+      </c>
+      <c r="F97" s="3">
+        <v>40360</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>460</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E98" s="1">
+        <v>59</v>
+      </c>
+      <c r="F98" s="3">
+        <v>40344</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>459</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E99" s="1">
+        <v>36</v>
+      </c>
+      <c r="F99" s="3">
+        <v>40331</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>458</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" s="1">
+        <v>54</v>
+      </c>
+      <c r="F100" s="3">
+        <v>40323</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>457</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E101" s="1">
+        <v>37</v>
+      </c>
+      <c r="F101" s="3">
+        <v>40317</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>456</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E102" s="1">
+        <v>41</v>
+      </c>
+      <c r="F102" s="3">
+        <v>40311</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>455</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E103" s="1">
+        <v>41</v>
+      </c>
+      <c r="F103" s="3">
+        <v>40310</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>454</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E104" s="1">
+        <v>40</v>
+      </c>
+      <c r="F104" s="3">
+        <v>40295</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>453</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E105" s="1">
+        <v>31</v>
+      </c>
+      <c r="F105" s="3">
+        <v>40290</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>452</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E106" s="1">
+        <v>34</v>
+      </c>
+      <c r="F106" s="3">
+        <v>40267</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>451</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E107" s="1">
+        <v>31</v>
+      </c>
+      <c r="F107" s="3">
+        <v>40248</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>450</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E108" s="1">
+        <v>32</v>
+      </c>
+      <c r="F108" s="3">
+        <v>40239</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>449</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E109" s="1">
+        <v>59</v>
+      </c>
+      <c r="F109" s="3">
+        <v>40190</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B50" r:id="rId1" tooltip="Last Statement of Jerry Martin" display="http://www.tdcj.state.tx.us/death_row/dr_info/martinjerrylast.html" xr:uid="{EFEFE5E1-9B6B-DD45-B744-4354C7407945}"/>
+    <hyperlink ref="B51" r:id="rId2" tooltip="Last Statement of Jamie McCoskey" display="http://www.tdcj.state.tx.us/death_row/dr_info/mccoskeyjamielast.html" xr:uid="{E40BB3E2-555E-4142-ADCB-BA175A1AB6DC}"/>
+    <hyperlink ref="B52" r:id="rId3" tooltip="Last Statement of Michael Yowell" display="http://www.tdcj.state.tx.us/death_row/dr_info/yowellmichaellast.html" xr:uid="{9D5B8C9F-E397-0C40-BD01-89402736370E}"/>
+    <hyperlink ref="B53" r:id="rId4" tooltip="Last Statement of Arturo Diaz" display="http://www.tdcj.state.tx.us/death_row/dr_info/diazarturolast.html" xr:uid="{AB8EA06E-5529-164B-94CE-05E35214F3C7}"/>
+    <hyperlink ref="B54" r:id="rId5" tooltip="Last Statement of Robert Garza" display="http://www.tdcj.state.tx.us/death_row/dr_info/garzarobertlast.html" xr:uid="{B0CE73AD-6A4E-F040-A66B-DC95A059D2FC}"/>
+    <hyperlink ref="B55" r:id="rId6" tooltip="Last Statement of Douglas Feldman" display="http://www.tdcj.state.tx.us/death_row/dr_info/feldmandouglaslast.html" xr:uid="{27A59B30-81C7-DB4A-9802-35E034F667DA}"/>
+    <hyperlink ref="B56" r:id="rId7" tooltip="Last Statement of Vaughn Ross" display="http://www.tdcj.state.tx.us/death_row/dr_info/rossvaughnlast.html" xr:uid="{8117F4BF-9416-F849-800D-2666748CD9B8}"/>
+    <hyperlink ref="B57" r:id="rId8" tooltip="Last Statement of John Quintanilla" display="http://www.tdcj.state.tx.us/death_row/dr_info/quintanillajohnlast.html" xr:uid="{0B03396A-81D8-E147-8140-E268CE31B534}"/>
+    <hyperlink ref="B58" r:id="rId9" tooltip="Last Statement of Kimberly McCarthy" display="http://www.tdcj.state.tx.us/death_row/dr_info/mccarthykimberlylast.html" xr:uid="{C02377B7-E42F-1D41-972B-E6C21D1B5399}"/>
+    <hyperlink ref="B59" r:id="rId10" tooltip="Last Statement of Elroy Chester" display="http://www.tdcj.state.tx.us/death_row/dr_info/chesterelroylast.html" xr:uid="{995506BB-86E6-7D42-9412-8D7F8270F44E}"/>
+    <hyperlink ref="B60" r:id="rId11" tooltip="Last Statement of Jeffrey Williams" display="http://www.tdcj.state.tx.us/death_row/dr_info/williamsjeffrey999350last.html" xr:uid="{5222354C-6AF3-DF49-A194-3A7F39989B70}"/>
+    <hyperlink ref="B61" r:id="rId12" tooltip="Last Statement of Carroll Parr" display="http://www.tdcj.state.tx.us/death_row/dr_info/parrcarrolllast.html" xr:uid="{BADC96B9-3696-CC4E-96E1-0BFE07D0F01E}"/>
+    <hyperlink ref="B62" r:id="rId13" tooltip="Last Statement of Richard Cobb" display="http://www.tdcj.state.tx.us/death_row/dr_info/cobbrichardlast.html" xr:uid="{6B03EF40-C715-1F4C-A188-03804A6F93AA}"/>
+    <hyperlink ref="B63" r:id="rId14" tooltip="Last Statement of Ronnie Threadgill" display="http://www.tdcj.state.tx.us/death_row/dr_info/threadgillronnielast.html" xr:uid="{550D51F4-0D88-5746-8B6F-D5445DF63356}"/>
+    <hyperlink ref="B64" r:id="rId15" tooltip="Last Statement of Rickey Lewis" display="http://www.tdcj.state.tx.us/death_row/dr_info/lewisrickeylast.html" xr:uid="{921B9806-8C33-2A48-98BF-9951CFD3AADF}"/>
+    <hyperlink ref="B65" r:id="rId16" tooltip="Last Statement of Carl Blue" display="http://www.tdcj.state.tx.us/death_row/dr_info/bluecarllast.html" xr:uid="{35EA8DAD-9C40-6344-A9E0-84516622BDBC}"/>
+    <hyperlink ref="B66" r:id="rId17" tooltip="Last Statement of Preston Hughes" display="http://www.tdcj.state.tx.us/death_row/dr_info/hughesprestonlast.html" xr:uid="{390041B2-53AD-F24D-9219-CA5BC10EBA8F}"/>
+    <hyperlink ref="B67" r:id="rId18" tooltip="Last Statement of Ramon Hernandez" display="http://www.tdcj.state.tx.us/death_row/dr_info/hernandezramontorreslast.html" xr:uid="{A5A3E9BD-1DD9-5C4C-9B67-0A77A23E25CF}"/>
+    <hyperlink ref="B68" r:id="rId19" tooltip="Last Statement of Mario Swain" display="http://www.tdcj.state.tx.us/death_row/dr_info/swainmariolast.html" xr:uid="{4130283E-5D78-EC47-ADA5-CACA916BA2C9}"/>
+    <hyperlink ref="B69" r:id="rId20" tooltip="Last Statement of Donnie Roberts, Jr." display="http://www.tdcj.state.tx.us/death_row/dr_info/robertsdonnielast.html" xr:uid="{141AC6A1-2A9D-2345-B65B-687D9FB49609}"/>
+    <hyperlink ref="B70" r:id="rId21" tooltip="Last Statement of Bobby Hines" display="http://www.tdcj.state.tx.us/death_row/dr_info/hinesbobbylast.html" xr:uid="{38A34415-6156-2C41-821E-10C1CBF92075}"/>
+    <hyperlink ref="B71" r:id="rId22" tooltip="Last Statement of Jonathan Green" display="http://www.tdcj.state.tx.us/death_row/dr_info/greenjonathanlast.html" xr:uid="{B8F62C1A-C486-B341-A5C0-3A1177B9923C}"/>
+    <hyperlink ref="B72" r:id="rId23" tooltip="Last Statement of Cleve Foster" display="http://www.tdcj.state.tx.us/death_row/dr_info/fosterclevelast.html" xr:uid="{68B53BD3-61C4-5242-9DEC-4B8E3136768B}"/>
+    <hyperlink ref="B73" r:id="rId24" tooltip="Last Statement of Robert Harris" display="http://www.tdcj.state.tx.us/death_row/dr_info/harrisrobertlast.html" xr:uid="{1E9E087A-AEC6-8247-AD43-C1E2E9DBB126}"/>
+    <hyperlink ref="B74" r:id="rId25" tooltip="Last Statement of Marvin Wilson" display="http://www.tdcj.state.tx.us/death_row/dr_info/wilsonmarvinlast.html" xr:uid="{561DF373-BB8D-F240-B6DB-306D3DDB486E}"/>
+    <hyperlink ref="B75" r:id="rId26" tooltip="Last Statement of Yokamon Hearn" display="http://www.tdcj.state.tx.us/death_row/dr_info/hearnyokamonlast.html" xr:uid="{BEC2FA02-04AF-D046-973F-FAAC604F8062}"/>
+    <hyperlink ref="B76" r:id="rId27" tooltip="Last Statement of Beunka Adams" display="http://www.tdcj.state.tx.us/death_row/dr_info/adamsbeunkalast.html" xr:uid="{4F0C6965-9693-A645-B450-44F8D73E3260}"/>
+    <hyperlink ref="B77" r:id="rId28" tooltip="Last Statement of Jesse Hernandez" display="http://www.tdcj.state.tx.us/death_row/dr_info/hernandezjesselast.html" xr:uid="{CE1A418A-6707-F048-B6A6-16BE88A7ACE4}"/>
+    <hyperlink ref="B78" r:id="rId29" tooltip="Last Statement of Keith Thurmond" display="http://www.tdcj.state.tx.us/death_row/dr_info/thurmondkeithlast.html" xr:uid="{2F6D9522-CD47-9341-B88C-33AAB19D976F}"/>
+    <hyperlink ref="B79" r:id="rId30" tooltip="Last Statement of George Rivas" display="http://www.tdcj.state.tx.us/death_row/dr_info/rivasgeorgelast.html" xr:uid="{87DD76AB-4F88-FC48-A9AF-8158F79E3136}"/>
+    <hyperlink ref="B80" r:id="rId31" tooltip="Last Statement of Rodrigo Hernandez" display="http://www.tdcj.state.tx.us/death_row/dr_info/hernandezrodrigolast.html" xr:uid="{2F48C8E8-2B7A-4C4C-834A-4D5FF529E6CC}"/>
+    <hyperlink ref="B81" r:id="rId32" tooltip="Last Statement of Guadalupe Esparza" display="http://www.tdcj.state.tx.us/death_row/dr_info/esparzaguadalupelast.html" xr:uid="{302A78E2-1222-DF40-9330-08AF6FB67A9D}"/>
+    <hyperlink ref="B82" r:id="rId33" tooltip="Last Statement of Frank Garcia" display="http://www.tdcj.state.tx.us/death_row/dr_info/garciafrankmlast.html" xr:uid="{54CBF7C9-6C63-2C4F-95BE-7F0307FB8346}"/>
+    <hyperlink ref="B83" r:id="rId34" tooltip="Last Statement of Lawrence Brewer" display="http://www.tdcj.state.tx.us/death_row/dr_info/brewerlawrencelast.html" xr:uid="{296C6EC7-0888-1B4A-92C2-8338FFA095FA}"/>
+    <hyperlink ref="B84" r:id="rId35" tooltip="Last Statement of Steven Woods" display="http://www.tdcj.state.tx.us/death_row/dr_info/woodsstevenlast.html" xr:uid="{9B2BE511-BE43-744A-B5D7-8072842E2F49}"/>
+    <hyperlink ref="B85" r:id="rId36" tooltip="Last Statement of Martin Robles" display="http://www.tdcj.state.tx.us/death_row/dr_info/roblesmartinlast.html" xr:uid="{26324669-7B8F-4340-91C7-DDC39B6630B8}"/>
+    <hyperlink ref="B86" r:id="rId37" tooltip="Last Statement of Mark Stroman" display="http://www.tdcj.state.tx.us/death_row/dr_info/stromanmarklast.html" xr:uid="{94DA8F5F-0EDD-5243-BA8E-522209F62FDC}"/>
+    <hyperlink ref="B87" r:id="rId38" tooltip="Last Statement of Humberto Leal" display="http://www.tdcj.state.tx.us/death_row/dr_info/lealhumbertolast.html" xr:uid="{081A508F-51F8-5940-9500-B9BBC2ECE254}"/>
+    <hyperlink ref="B88" r:id="rId39" tooltip="Last Statement of Milton Mathis" display="http://www.tdcj.state.tx.us/death_row/dr_info/mathismiltonlast.html" xr:uid="{B6158731-9C3D-CC45-A75B-F28F8AA0DF0A}"/>
+    <hyperlink ref="B89" r:id="rId40" tooltip="Last Statement of Lee Taylor" display="http://www.tdcj.state.tx.us/death_row/dr_info/taylorleelast.html" xr:uid="{D4B84DB5-3390-4946-8334-19A8153E55FA}"/>
+    <hyperlink ref="B90" r:id="rId41" tooltip="Last Statement of Gayland Bradford" display="http://www.tdcj.state.tx.us/death_row/dr_info/bradfordgaylandlast.html" xr:uid="{2D7D4360-0E69-9443-8DA7-7D20476892D7}"/>
+    <hyperlink ref="B91" r:id="rId42" tooltip="Last Statement of Cary Kerr" display="http://www.tdcj.state.tx.us/death_row/dr_info/kerrcarylast.html" xr:uid="{88FDB004-E7B3-4242-99E5-82838F2F7310}"/>
+    <hyperlink ref="B92" r:id="rId43" tooltip="Last Statement of Timothy Adams" display="http://www.tdcj.state.tx.us/death_row/dr_info/no_last_statement.html" xr:uid="{1D0C9966-2470-344F-B8BE-398AA2DCA4E8}"/>
+    <hyperlink ref="B93" r:id="rId44" tooltip="Last Statement of Michael Hall" display="http://www.tdcj.state.tx.us/death_row/dr_info/hallmichaellast.html" xr:uid="{1C7A0C55-9BC1-B94D-B049-9BFAC64A8089}"/>
+    <hyperlink ref="B94" r:id="rId45" tooltip="Last Statement of Larry Wooten" display="http://www.tdcj.state.tx.us/death_row/dr_info/wootenlarrylast.html" xr:uid="{8FA25BE3-F328-ED4C-8076-A0AFFD31C342}"/>
+    <hyperlink ref="B95" r:id="rId46" tooltip="Last Statement of Peter Cantu" display="http://www.tdcj.state.tx.us/death_row/dr_info/cantupeterlast.html" xr:uid="{BC67FADF-27D5-E647-A50E-86D7D5CE2CEA}"/>
+    <hyperlink ref="B96" r:id="rId47" tooltip="Last Statement of Derrick Jackson" display="http://www.tdcj.state.tx.us/death_row/dr_info/jacksonderricklast.html" xr:uid="{8EEDB423-E068-D745-9EAE-6F9F6724CDDA}"/>
+    <hyperlink ref="B97" r:id="rId48" tooltip="Last Statement of Michael Perry" display="http://www.tdcj.state.tx.us/death_row/dr_info/perrymichaellast.html" xr:uid="{A5356676-2B69-7A43-967C-652A128325ED}"/>
+    <hyperlink ref="B98" r:id="rId49" tooltip="Last Statement of David Powell" display="http://www.tdcj.state.tx.us/death_row/dr_info/no_last_statement.html" xr:uid="{55E05824-F255-5F44-BBD8-E95778CAA249}"/>
+    <hyperlink ref="B99" r:id="rId50" tooltip="Last Statement of George Jones" display="http://www.tdcj.state.tx.us/death_row/dr_info/jonesgeorgelast.html" xr:uid="{F4F820F7-3BF8-4740-AB57-D7C13AB5CB21}"/>
+    <hyperlink ref="B100" r:id="rId51" tooltip="Last Statement of John Alba" display="http://www.tdcj.state.tx.us/death_row/dr_info/albajohnlast.html" xr:uid="{45161E94-D537-CF44-AC4D-F0A87E8D3BC9}"/>
+    <hyperlink ref="B101" r:id="rId52" tooltip="Last Statement of Rogelio Cannady" display="http://www.tdcj.state.tx.us/death_row/dr_info/cannadyrogeliolast.html" xr:uid="{41EB8500-E1F3-C943-8096-78DD77A47F1C}"/>
+    <hyperlink ref="B102" r:id="rId53" tooltip="Last Statement of Billy Galloway" display="http://www.tdcj.state.tx.us/death_row/dr_info/gallowaybillylast.html" xr:uid="{6573E4D1-8CE2-7D44-B620-8C0938A4A320}"/>
+    <hyperlink ref="B103" r:id="rId54" tooltip="Last Statement of Kevin Varga" display="http://www.tdcj.state.tx.us/death_row/dr_info/vargakevinlast.html" xr:uid="{D7DD362D-F948-0E45-9CFF-807C8651BF32}"/>
+    <hyperlink ref="B104" r:id="rId55" tooltip="Last Statement of Samuel Bustamante" display="http://www.tdcj.state.tx.us/death_row/dr_info/no_last_statement.html" xr:uid="{CBC3D649-17A9-F94D-831C-BBD8526F0976}"/>
+    <hyperlink ref="B105" r:id="rId56" tooltip="Last Statement of William Berkley" display="http://www.tdcj.state.tx.us/death_row/dr_info/berkleywilliamlast.html" xr:uid="{6AEC93AD-A788-4242-BB91-CA93E04675E7}"/>
+    <hyperlink ref="B106" r:id="rId57" tooltip="Last Statement of Franklin Alix" display="http://www.tdcj.state.tx.us/death_row/dr_info/alixfranklinlast.html" xr:uid="{D3BD416F-ECDD-2245-8EEA-53797FADB9EA}"/>
+    <hyperlink ref="B107" r:id="rId58" tooltip="Last Statement of Joshua Maxwell" display="http://www.tdcj.state.tx.us/death_row/dr_info/maxwelljoshualast.html" xr:uid="{41DD9340-D938-DB45-BC95-589A21104E63}"/>
+    <hyperlink ref="B108" r:id="rId59" tooltip="Last Statement of Michael Sigala" display="http://www.tdcj.state.tx.us/death_row/dr_info/sigalamichaellast.html" xr:uid="{2A3345F8-35CB-384D-B7BE-C7C4241C1FEF}"/>
+    <hyperlink ref="B109" r:id="rId60" tooltip="Last Statement of Gary Johnson" display="http://www.tdcj.state.tx.us/death_row/dr_info/johnsongarylast.html" xr:uid="{210470B0-7B7B-8948-A167-8EFB5D873B45}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFA9DAB-77C6-9347-9234-D0F30ADA75E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>